<commit_message>
add example image_tags xls
</commit_message>
<xml_diff>
--- a/python/image_tags.xlsx
+++ b/python/image_tags.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>image_uuid</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -230,6 +230,10 @@
   <si>
     <t>CentOS 7.5 64bit</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -303,13 +307,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -614,214 +621,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="41.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update image_tags no 6c23 uuid
</commit_message>
<xml_diff>
--- a/python/image_tags.xlsx
+++ b/python/image_tags.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>image_uuid</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -36,9 +36,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>InImage-inspurtest13-0000000015</t>
-  </si>
-  <si>
     <t>InImage-jiyouai-0000000016</t>
   </si>
   <si>
@@ -126,10 +123,6 @@
   </si>
   <si>
     <t>1aa57b3e-e483-47b8-af5a-71448be18d78</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6c23b1b2-5b65-4d3e-847f-ca28e36d6cbc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -559,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -591,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -604,42 +597,42 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>30</v>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>31</v>
+      <c r="B4" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
+      <c r="B5" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -647,13 +640,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
@@ -661,13 +654,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
@@ -675,13 +668,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
@@ -689,13 +682,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
@@ -705,11 +698,11 @@
       <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>20</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
@@ -717,27 +710,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>